<commit_message>
enforce list membership, and HPC version of process script
</commit_message>
<xml_diff>
--- a/RBMSgenre_forHenry All Columns-Sample-10.xlsx
+++ b/RBMSgenre_forHenry All Columns-Sample-10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hls19\Desktop\RE_ Notes from our meeting today - GenAI Library Network\tufts-libraries-metadata-gen-ai-group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D942C345-D50F-4A6E-B473-B2C8DC72E84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1BE8FCF-D1F3-46EB-96B0-29BB87FE86C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC55C20B-D39B-4347-AD4E-D547C99BC8ED}"/>
   </bookViews>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6560C7DA-44DC-4352-80AD-8B858B0AD816}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>